<commit_message>
Reorder columns databases export
#654 Co-authored-by: uortiz <uortiz@sorint.it>
</commit_message>
<xml_diff>
--- a/resources/templates/template_databases.xlsx
+++ b/resources/templates/template_databases.xlsx
@@ -1,52 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raf\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD06E9E9-BF5F-4146-BFDD-E73A7C4DBFA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{08E96F0B-B0E9-4384-9D3A-EFB7CBF32CD2}"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Databases" sheetId="1" r:id="rId1"/>
+    <sheet name="Databases" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
-    <t>DB Name</t>
-  </si>
-  <si>
-    <t>Unique name</t>
-  </si>
-  <si>
-    <t>Database version</t>
+    <t xml:space="preserve">DB Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unique name</t>
   </si>
   <si>
     <t>Hostname</t>
   </si>
   <si>
+    <t xml:space="preserve">Database version</t>
+  </si>
+  <si>
     <t>Status</t>
   </si>
   <si>
@@ -62,19 +42,19 @@
     <t>Blocksize</t>
   </si>
   <si>
-    <t>CPU Count</t>
+    <t xml:space="preserve">CPU Count</t>
   </si>
   <si>
     <t>Work</t>
   </si>
   <si>
-    <t>Memory used</t>
-  </si>
-  <si>
-    <t>Datafile GB</t>
-  </si>
-  <si>
-    <t>Segment GB</t>
+    <t xml:space="preserve">Memory used</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Datafile GB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Segment GB</t>
   </si>
   <si>
     <t>Archivelog</t>
@@ -92,21 +72,19 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2">
     <font>
-      <sz val="11"/>
+      <name val="Calibri"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <sz val="11.000000"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Calibri"/>
       <b/>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <sz val="11.000000"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -128,11 +106,11 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -145,15 +123,295 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
   </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Angsana New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ 明朝"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Cordia New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Tema di Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -195,108 +453,14 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
+        <a:latin typeface="Calibri Light"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -304,7 +468,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -330,7 +494,7 @@
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -382,16 +546,28 @@
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -407,7 +583,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -438,44 +614,37 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B58A2885-5B19-41A0-86EA-2ABE6059BF6E}">
-  <dimension ref="A1:R1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView workbookViewId="0" zoomScale="100">
+      <selection activeCell="D35" activeCellId="0" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col bestFit="1" customWidth="1" min="2" max="2" width="14.18359375"/>
+    <col customWidth="1" min="3" max="3" width="14.18359375"/>
+    <col bestFit="1" customWidth="1" min="4" max="4" width="17.453125"/>
+    <col bestFit="1" customWidth="1" min="5" max="5" width="6.42578125"/>
+    <col bestFit="1" customWidth="1" min="6" max="6" width="12.42578125"/>
+    <col bestFit="1" customWidth="1" min="7" max="7" width="8.42578125"/>
+    <col bestFit="1" customWidth="1" min="8" max="8" width="7.7109375"/>
+    <col bestFit="1" customWidth="1" min="10" max="10" width="10.42578125"/>
+    <col bestFit="1" customWidth="1" min="11" max="11" width="5.85546875"/>
+    <col bestFit="1" customWidth="1" min="12" max="12" width="13.42578125"/>
+    <col bestFit="1" customWidth="1" min="13" max="13" width="11"/>
+    <col bestFit="1" customWidth="1" min="14" max="14" width="11.85546875"/>
+    <col bestFit="1" customWidth="1" min="15" max="15" width="10.42578125"/>
+    <col bestFit="1" customWidth="1" min="16" max="16" width="3.42578125"/>
+    <col bestFit="1" customWidth="1" min="17" max="17" width="4.5703125"/>
+    <col bestFit="1" customWidth="1" min="18" max="18" width="3.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" ht="30" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -532,7 +701,9 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup blackAndWhite="0" cellComments="none" copies="1" draft="0" errors="displayed" firstPageNumber="-1" fitToHeight="1" fitToWidth="1" horizontalDpi="600" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="1" verticalDpi="600"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added pgsql migrability export
</commit_message>
<xml_diff>
--- a/resources/templates/template_databases.xlsx
+++ b/resources/templates/template_databases.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t xml:space="preserve">DB Name</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t xml:space="preserve">PDBs </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pgsql Migrability</t>
   </si>
 </sst>
 </file>
@@ -163,13 +166,21 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -185,96 +196,100 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:U1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="U7" activeCellId="0" sqref="U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="14.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="8.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="5.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="10.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="11.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="10.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="3.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="4.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="3.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="10.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="14.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="6.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="12.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="8.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="7.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="10.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="5.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="13.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="10.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="11.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="10.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="3.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="4.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="3.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="10.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="14.96"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="2" t="s">
         <v>19</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added clusterware version to oracle db API
</commit_message>
<xml_diff>
--- a/resources/templates/template_databases.xlsx
+++ b/resources/templates/template_databases.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t xml:space="preserve">DB Name</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t xml:space="preserve">Pgsql Migrability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clusterware Version</t>
   </si>
 </sst>
 </file>
@@ -166,7 +169,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -179,8 +182,12 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -200,10 +207,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U1"/>
+  <dimension ref="A1:V1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U7" activeCellId="0" sqref="U7"/>
+      <selection pane="topLeft" activeCell="V1" activeCellId="0" sqref="V1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -224,7 +231,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="4.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="3.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="10.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="14.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="14.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="18.23"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -290,6 +298,9 @@
       </c>
       <c r="U1" s="3" t="s">
         <v>20</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Open oracle db list xlsx to the first cell
</commit_message>
<xml_diff>
--- a/resources/templates/template_databases.xlsx
+++ b/resources/templates/template_databases.xlsx
@@ -95,7 +95,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -116,6 +116,13 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="0"/>
     </font>
     <font>
@@ -182,12 +189,12 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -209,8 +216,8 @@
   </sheetPr>
   <dimension ref="A1:V1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="V1" activeCellId="0" sqref="V1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -232,74 +239,74 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="3.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="10.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="14.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="18.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="18.23"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="S1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="T1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="U1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="V1" s="3" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added dbID to oracle db API export
</commit_message>
<xml_diff>
--- a/resources/templates/template_databases.xlsx
+++ b/resources/templates/template_databases.xlsx
@@ -20,12 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t xml:space="preserve">DB Name</t>
   </si>
   <si>
     <t xml:space="preserve">Unique name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Db ID</t>
   </si>
   <si>
     <t xml:space="preserve">Hostname</t>
@@ -95,7 +98,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -116,13 +119,6 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
       <family val="0"/>
     </font>
     <font>
@@ -176,7 +172,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -189,11 +185,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -214,100 +206,103 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V1"/>
+  <dimension ref="A1:W1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="14.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="6.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="12.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="8.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="7.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="10.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="5.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="13.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="10.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="11.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="10.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="3.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="4.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="3.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="10.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="14.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="18.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="1" width="14.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="6.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="8.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="7.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="10.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="5.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="13.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="10.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="11.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="10.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="3.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="4.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="3.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="10.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="14.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="18.23"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="U1" s="2" t="s">
         <v>20</v>
       </c>
       <c r="V1" s="3" t="s">
         <v>21</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated db list & host list exports
</commit_message>
<xml_diff>
--- a/resources/templates/template_databases.xlsx
+++ b/resources/templates/template_databases.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t xml:space="preserve">DB Name</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t xml:space="preserve">Clusterware Version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Role</t>
   </si>
 </sst>
 </file>
@@ -206,10 +209,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:W1"/>
+  <dimension ref="A1:X1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="X1" activeCellId="0" sqref="X1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -304,6 +307,9 @@
       <c r="W1" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="X1" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Removed withespace in oracle db export
</commit_message>
<xml_diff>
--- a/resources/templates/template_databases.xlsx
+++ b/resources/templates/template_databases.xlsx
@@ -79,10 +79,10 @@
     <t xml:space="preserve">HA</t>
   </si>
   <si>
-    <t xml:space="preserve">Pluggable  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">PDBs </t>
+    <t xml:space="preserve">Pluggable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PDBs</t>
   </si>
   <si>
     <t xml:space="preserve">Pgsql Migrability</t>
@@ -211,8 +211,8 @@
   </sheetPr>
   <dimension ref="A1:X1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="X1" activeCellId="0" sqref="X1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T1" activeCellId="0" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Updated API response & added policies audit to db export
</commit_message>
<xml_diff>
--- a/resources/templates/template_databases.xlsx
+++ b/resources/templates/template_databases.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t xml:space="preserve">DB Name</t>
   </si>
@@ -92,6 +92,9 @@
   </si>
   <si>
     <t xml:space="preserve">Role</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Policies Audit</t>
   </si>
 </sst>
 </file>
@@ -209,10 +212,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:X1"/>
+  <dimension ref="A1:Y1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T1" activeCellId="0" sqref="T1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -235,6 +238,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="10.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="14.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="18.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="12.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -309,6 +314,9 @@
       </c>
       <c r="X1" s="2" t="s">
         <v>23</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated oracle db list export API
</commit_message>
<xml_diff>
--- a/resources/templates/template_databases.xlsx
+++ b/resources/templates/template_databases.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t xml:space="preserve">DB Name</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t xml:space="preserve">Policies Audit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Services</t>
   </si>
 </sst>
 </file>
@@ -212,7 +215,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y1"/>
+  <dimension ref="A1:Z1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -238,8 +241,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="10.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="14.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="18.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="12.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="12.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -317,6 +320,9 @@
       </c>
       <c r="Y1" s="2" t="s">
         <v>24</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>